<commit_message>
progress on laser control
</commit_message>
<xml_diff>
--- a/monet/tests/TestData/calibrate/power_database.xlsx
+++ b/monet/tests/TestData/calibrate/power_database.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>18:44</t>
+          <t>20:02</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.881267938455818</v>
+        <v>0.6458351956601358</v>
       </c>
       <c r="G2" t="n">
-        <v>98.00743824697096</v>
+        <v>98.52574419339665</v>
       </c>
       <c r="H2" t="n">
-        <v>100.0840763066397</v>
+        <v>99.81316567335617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored and resolved test issues
</commit_message>
<xml_diff>
--- a/monet/tests/TestData/calibrate/power_database.xlsx
+++ b/monet/tests/TestData/calibrate/power_database.xlsx
@@ -489,22 +489,22 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>2022-07-20</t>
+          <t>2022-07-22</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>20:02</t>
+          <t>11:36</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.6458351956601358</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>98.52574419339665</v>
+        <v>99.15573139735331</v>
       </c>
       <c r="H2" t="n">
-        <v>99.81316567335617</v>
+        <v>100.4527343703501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PointCurveAnalyzer in case no Attenuation is possible
</commit_message>
<xml_diff>
--- a/monet/tests/TestData/calibrate/power_database.xlsx
+++ b/monet/tests/TestData/calibrate/power_database.xlsx
@@ -515,17 +515,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>198.9363304828388</v>
+        <v>200.9472680245446</v>
       </c>
       <c r="H2" t="n">
-        <v>100.1092048644831</v>
+        <v>99.93525306664431</v>
       </c>
     </row>
     <row r="3">
@@ -541,17 +541,17 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.6541127318825524</v>
+        <v>4.035040301886283e-09</v>
       </c>
       <c r="G3" t="n">
-        <v>397.8270337381952</v>
+        <v>397.8932912197835</v>
       </c>
       <c r="H3" t="n">
-        <v>85.09536083379551</v>
+        <v>85.10312446386273</v>
       </c>
     </row>
     <row r="4">
@@ -567,17 +567,17 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2.818838495954878e-10</v>
+        <v>0.7327678547907854</v>
       </c>
       <c r="G4" t="n">
-        <v>1000.681264839615</v>
+        <v>998.3112709787323</v>
       </c>
       <c r="H4" t="n">
-        <v>70.07847949434861</v>
+        <v>69.99392331902639</v>
       </c>
     </row>
     <row r="5">
@@ -595,17 +595,17 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.8649512840980516</v>
+        <v>0.5913465965666089</v>
       </c>
       <c r="G5" t="n">
-        <v>400.4756477737629</v>
+        <v>400.5308692093085</v>
       </c>
       <c r="H5" t="n">
-        <v>55.10294499167115</v>
+        <v>54.90910915961167</v>
       </c>
     </row>
     <row r="6">
@@ -621,17 +621,17 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.1292369591466371</v>
+        <v>0.6392115640936014</v>
       </c>
       <c r="G6" t="n">
-        <v>998.9516406384713</v>
+        <v>998.8757817610992</v>
       </c>
       <c r="H6" t="n">
-        <v>129.9875440163075</v>
+        <v>130.0015809752132</v>
       </c>
     </row>
     <row r="7">
@@ -647,17 +647,17 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>15:44</t>
+          <t>16:16</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2.966749268473734e-08</v>
+        <v>0.8295477617416493</v>
       </c>
       <c r="G7" t="n">
-        <v>2000.321852598102</v>
+        <v>1999.605449741923</v>
       </c>
       <c r="H7" t="n">
-        <v>115.010997765126</v>
+        <v>114.9985694223957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>